<commit_message>
fixed weekly questions tab
</commit_message>
<xml_diff>
--- a/data/east/Survivor_49_East.xlsx
+++ b/data/east/Survivor_49_East.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\east\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28017F14-F2A1-4C5B-9BDA-1BF510A52F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4719AFA-0406-4524-8BBA-A9D5C7441980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{446E4F7A-E405-E54E-8316-75643DDCCDA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{446E4F7A-E405-E54E-8316-75643DDCCDA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoreboard_Table" sheetId="5" r:id="rId1"/>
@@ -774,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -841,7 +841,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3031,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BD0539-AEEA-4F66-B012-77D12D726F3A}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3656,22 +3655,22 @@
       <c r="D18" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="54" t="s">
         <v>64</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="59" t="s">
+      <c r="H18" s="58" t="s">
         <v>96</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J18" s="55" t="s">
+      <c r="J18" s="54" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3679,7 +3678,7 @@
       <c r="A19" s="33">
         <v>4</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="51" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="48" t="s">
@@ -3688,22 +3687,22 @@
       <c r="D19" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="56" t="s">
+      <c r="G19" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="H19" s="59" t="s">
+      <c r="H19" s="58" t="s">
         <v>44</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J19" s="56" t="s">
+      <c r="J19" s="55" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3714,28 +3713,28 @@
       <c r="B20" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="52" t="s">
         <v>92</v>
       </c>
       <c r="D20" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="57" t="s">
+      <c r="G20" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="H20" s="61" t="s">
+      <c r="H20" s="60" t="s">
         <v>92</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="57" t="s">
+      <c r="J20" s="56" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3746,28 +3745,28 @@
       <c r="B21" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="52" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="60" t="s">
+      <c r="F21" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="56" t="s">
+      <c r="G21" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="H21" s="59" t="s">
+      <c r="H21" s="58" t="s">
         <v>92</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J21" s="56" t="s">
+      <c r="J21" s="55" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3778,28 +3777,28 @@
       <c r="B22" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="52" t="s">
         <v>92</v>
       </c>
       <c r="D22" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="57" t="s">
+      <c r="G22" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="H22" s="61" t="s">
+      <c r="H22" s="60" t="s">
         <v>92</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J22" s="57" t="s">
+      <c r="J22" s="56" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3813,25 +3812,25 @@
       <c r="C23" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="58" t="s">
+      <c r="F23" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="58" t="s">
         <v>97</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J23" s="58" t="s">
+      <c r="J23" s="57" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3864,8 +3863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1227AA98-08EE-4642-87CC-39AAE2D5BB8A}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3900,19 +3899,19 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="62">
+      <c r="B2" s="61">
         <v>0</v>
       </c>
-      <c r="C2" s="62">
-        <v>2</v>
-      </c>
-      <c r="D2" s="62">
+      <c r="C2" s="61">
+        <v>2</v>
+      </c>
+      <c r="D2" s="61">
         <v>0</v>
       </c>
-      <c r="E2" s="62">
-        <v>2</v>
-      </c>
-      <c r="F2" s="62">
+      <c r="E2" s="61">
+        <v>2</v>
+      </c>
+      <c r="F2" s="61">
         <v>0</v>
       </c>
       <c r="G2" s="10">
@@ -3923,19 +3922,19 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B3" s="61">
         <v>4</v>
       </c>
-      <c r="C3" s="62">
-        <v>2</v>
-      </c>
-      <c r="D3" s="62">
-        <v>2</v>
-      </c>
-      <c r="E3" s="62">
-        <v>1</v>
-      </c>
-      <c r="F3" s="62">
+      <c r="C3" s="61">
+        <v>2</v>
+      </c>
+      <c r="D3" s="61">
+        <v>2</v>
+      </c>
+      <c r="E3" s="61">
+        <v>1</v>
+      </c>
+      <c r="F3" s="61">
         <v>0</v>
       </c>
       <c r="G3" s="10">
@@ -3946,19 +3945,19 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="62">
-        <v>2</v>
-      </c>
-      <c r="C4" s="62">
-        <v>1</v>
-      </c>
-      <c r="D4" s="62">
+      <c r="B4" s="61">
+        <v>2</v>
+      </c>
+      <c r="C4" s="61">
+        <v>1</v>
+      </c>
+      <c r="D4" s="61">
         <v>3</v>
       </c>
-      <c r="E4" s="62">
-        <v>2</v>
-      </c>
-      <c r="F4" s="62">
+      <c r="E4" s="61">
+        <v>2</v>
+      </c>
+      <c r="F4" s="61">
         <v>0</v>
       </c>
       <c r="G4" s="10">
@@ -3969,22 +3968,22 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="61">
         <v>3</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="61">
         <v>3</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="61">
         <v>3</v>
       </c>
-      <c r="E5" s="50">
-        <v>2</v>
-      </c>
-      <c r="F5" s="50">
+      <c r="E5" s="61">
+        <v>2</v>
+      </c>
+      <c r="F5" s="61">
         <v>0</v>
       </c>
-      <c r="G5" s="50">
+      <c r="G5" s="61">
         <v>3</v>
       </c>
     </row>

</xml_diff>